<commit_message>
Planilha alterada com exemplo
</commit_message>
<xml_diff>
--- a/datasets/PEP-2017/2017-05-04T23-49-06_SINTESE_bridges_cleaned.xlsx
+++ b/datasets/PEP-2017/2017-05-04T23-49-06_SINTESE_bridges_cleaned.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Annotations per class" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Nova geração (09-05-18)" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="387">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -1145,6 +1146,42 @@
   </si>
   <si>
     <t xml:space="preserve">Total Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource (Instance/Class)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Direct Hits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Indirect hits (type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Indirect hits (subclass)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dbpedia.org/resource/Magazine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dbpedia.org/ontology/Magazine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magazine</t>
   </si>
 </sst>
 </file>
@@ -1526,8 +1563,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.137590520078999"/>
-          <c:y val="0.0166666666666667"/>
+          <c:x val="0.137601867275792"/>
+          <c:y val="0.0167154594390405"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1539,10 +1576,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0342330480579328"/>
-          <c:y val="0.112492433766355"/>
-          <c:w val="0.934067468629681"/>
-          <c:h val="0.592401173348233"/>
+          <c:x val="0.034233389524503"/>
+          <c:y val="0.112475210123713"/>
+          <c:w val="0.934056836204403"/>
+          <c:h val="0.592359996222495"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2253,11 +2290,11 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="0"/>
-        <c:axId val="47982789"/>
-        <c:axId val="50913140"/>
+        <c:axId val="58737888"/>
+        <c:axId val="44696552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47982789"/>
+        <c:axId val="58737888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2289,14 +2326,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50913140"/>
+        <c:crossAx val="44696552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50913140"/>
+        <c:axId val="44696552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="53000"/>
@@ -2337,7 +2374,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47982789"/>
+        <c:crossAx val="58737888"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2405,13 +2442,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>61</xdr:col>
-      <xdr:colOff>417960</xdr:colOff>
+      <xdr:colOff>417600</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2419,8 +2456,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8322840" y="434520"/>
-        <a:ext cx="36091080" cy="7624080"/>
+        <a:off x="8322840" y="434880"/>
+        <a:ext cx="36090720" cy="7623360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2440,8 +2477,8 @@
   </sheetPr>
   <dimension ref="A1:C366"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A1:E1 A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3129,15 +3166,16 @@
         <v>380</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
         <v>76</v>
       </c>
       <c r="B67" s="7" t="n">
         <v>379</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="0"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
         <v>77</v>
       </c>
@@ -5539,4 +5577,123 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>